<commit_message>
update create variables, final data set, and add linear regression
</commit_message>
<xml_diff>
--- a/output/Data_Dictionary.xlsx
+++ b/output/Data_Dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RProjects\github\toothheart\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RProjects\github\toothheart\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFCC71F-ACFE-43A1-AEBC-BED1BD1DF6AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742844D7-8D59-4E49-870A-81BB4503DFB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16950" yWindow="-15705" windowWidth="23550" windowHeight="14385" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="780" windowWidth="25980" windowHeight="14385" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="232">
   <si>
     <t>Fieldname</t>
   </si>
@@ -106,9 +106,6 @@
     <t>AGE3</t>
   </si>
   <si>
-    <t>AGE4</t>
-  </si>
-  <si>
     <t>MALE</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>INC4</t>
   </si>
   <si>
-    <t>INC5</t>
-  </si>
-  <si>
     <t>UNDWT</t>
   </si>
   <si>
@@ -280,9 +274,6 @@
     <t>Refused/missing</t>
   </si>
   <si>
-    <t>NEVERSMK</t>
-  </si>
-  <si>
     <t>_HISPANC</t>
   </si>
   <si>
@@ -317,12 +308,6 @@
   </si>
   <si>
     <t>EDGRP</t>
-  </si>
-  <si>
-    <t>HIGHSCOOL</t>
-  </si>
-  <si>
-    <t>SOMECOL</t>
   </si>
   <si>
     <t>COLLEGE</t>
@@ -455,9 +440,6 @@
     <t>Removed</t>
   </si>
   <si>
-    <t>ALLTEETH</t>
-  </si>
-  <si>
     <t>MOSTTEETH</t>
   </si>
   <si>
@@ -512,9 +494,6 @@
     <t>Flag for 6 or more teeth removed</t>
   </si>
   <si>
-    <t xml:space="preserve">Flag for no teeth removed </t>
-  </si>
-  <si>
     <t>Flag for all teeth removed</t>
   </si>
   <si>
@@ -527,9 +506,6 @@
     <t>Hispanic, Latino/a, or Spanish origin calculated variable</t>
   </si>
   <si>
-    <t>1=hispanic, 2=not hispanic</t>
-  </si>
-  <si>
     <t>Calculated multiracial race categorization</t>
   </si>
   <si>
@@ -546,9 +522,6 @@
   </si>
   <si>
     <t>_AGEG5YR</t>
-  </si>
-  <si>
-    <t>Flag for participants 50 to 59</t>
   </si>
   <si>
     <t>Flag for participants 60 to 69</t>
@@ -588,9 +561,6 @@
 Age &gt; 79</t>
   </si>
   <si>
-    <t>HIGHSCHOOOL</t>
-  </si>
-  <si>
     <t>SEX2 Descripton</t>
   </si>
   <si>
@@ -624,9 +594,6 @@
     <t>1=never attended through grade 11, 0=all others</t>
   </si>
   <si>
-    <t>1=high school graduate or GED, 0=all others</t>
-  </si>
-  <si>
     <t>1=attended college or technical school, 0=all others</t>
   </si>
   <si>
@@ -666,9 +633,6 @@
     <t>1=$35k - &lt;$50k, 0=all others</t>
   </si>
   <si>
-    <t>1=$50K+, 0=all others</t>
-  </si>
-  <si>
     <t>BMICAT Description</t>
   </si>
   <si>
@@ -717,9 +681,6 @@
     <t>Cleaned up version of BMI5CAT</t>
   </si>
   <si>
-    <t>1=never smoked, 0=all others</t>
-  </si>
-  <si>
     <t>1=former smoker, 0=all others</t>
   </si>
   <si>
@@ -781,6 +742,21 @@
   </si>
   <si>
     <t>NODIABETE</t>
+  </si>
+  <si>
+    <t>HISPANC2</t>
+  </si>
+  <si>
+    <t>1=hispanic, 0=not hispanic</t>
+  </si>
+  <si>
+    <t>Cleaned up version of HISPANC</t>
+  </si>
+  <si>
+    <t>RMTETH4</t>
+  </si>
+  <si>
+    <t>SOMECOLl</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1276,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1336,359 +1312,357 @@
     </row>
     <row r="2" spans="1:5" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>152</v>
+      <c r="C6" s="6" t="s">
+        <v>144</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="19" t="s">
+      <c r="C10" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>84</v>
+      <c r="E10" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>141</v>
+        <v>21</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="C13" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>155</v>
+      <c r="E13" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>14</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
-        <v>157</v>
+        <v>228</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1699,13 +1673,13 @@
         <v>14</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1716,558 +1690,518 @@
         <v>14</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D25" s="6" t="s">
+      <c r="C26" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>41</v>
+      <c r="E26" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>43</v>
+        <v>231</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="D30" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="D30" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>41</v>
+      <c r="E30" s="19" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>189</v>
+      <c r="C31" s="7" t="s">
+        <v>185</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="D32" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="19" t="s">
-        <v>45</v>
+      <c r="E32" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C33" s="7" t="s">
-        <v>196</v>
+      <c r="C33" s="16" t="s">
+        <v>187</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="D36" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="D36" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>45</v>
+      <c r="E36" s="19" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="16" t="s">
-        <v>200</v>
+      <c r="C37" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="16" t="s">
-        <v>201</v>
-      </c>
-      <c r="D38" s="6" t="s">
+      <c r="C39" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>113</v>
+      <c r="E39" s="6" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>95</v>
+        <v>226</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
-        <v>87</v>
+        <v>133</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>98</v>
+        <v>139</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>239</v>
+        <v>91</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="D44" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E44" s="19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="6" t="s">
+      <c r="E44" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E45" s="6" t="s">
-        <v>114</v>
+      <c r="E45" s="18" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>114</v>
+      <c r="E46" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E47" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" s="6" t="s">
+      <c r="E47" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D48" s="6" t="s">
+      <c r="C49" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E48" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E49" s="18" t="s">
-        <v>74</v>
+      <c r="E49" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="D52" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D52" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E52" s="18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="E52" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="6"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="6"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="6"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="6"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
@@ -2317,34 +2251,6 @@
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
       <c r="E86" s="6"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="6"/>
-      <c r="B87" s="6"/>
-      <c r="C87" s="6"/>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="6"/>
-      <c r="B88" s="6"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="6"/>
-      <c r="E88" s="6"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="6"/>
-      <c r="B89" s="6"/>
-      <c r="C89" s="6"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="6"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="6"/>
-      <c r="B90" s="6"/>
-      <c r="C90" s="6"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2373,19 +2279,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2399,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="E2" s="10">
         <v>0</v>
@@ -2416,7 +2322,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E3" s="10">
         <v>1</v>
@@ -2427,13 +2333,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C4" s="10">
         <v>9</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2462,19 +2368,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2488,7 +2394,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="E2" s="10">
         <v>0</v>
@@ -2499,13 +2405,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C3" s="10">
         <v>0</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="E3" s="10">
         <v>1</v>
@@ -2522,7 +2428,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2530,13 +2436,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C5" s="10">
         <v>9</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2544,13 +2450,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C6" s="10">
         <v>9</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2564,7 +2470,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2575,7 +2481,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2586,11 +2492,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2598,151 +2502,135 @@
     <col min="2" max="2" width="32.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="12.42578125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="12"/>
+    <col min="5" max="5" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12.42578125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="12" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="C2" s="12">
         <v>2</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="E2" s="12">
         <v>0</v>
       </c>
       <c r="F2" s="12">
-        <v>0</v>
-      </c>
-      <c r="G2" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="C3" s="12">
         <v>2</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="E3" s="12">
         <v>0</v>
       </c>
       <c r="F3" s="12">
-        <v>0</v>
-      </c>
-      <c r="G3" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C4" s="12">
         <v>1</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="E4" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="12">
-        <v>1</v>
-      </c>
-      <c r="G4" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="C5" s="12">
         <v>0</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="E5" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="12">
         <v>0</v>
       </c>
-      <c r="G5" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>9</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C6" s="12">
         <v>9</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J16" s="5"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2771,19 +2659,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2825,13 +2713,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="12">
         <v>9</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2839,13 +2727,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="12">
         <v>9</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2877,25 +2765,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2903,13 +2791,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E2" s="12">
         <v>1</v>
@@ -2926,13 +2814,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="C3" s="12">
         <v>1</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="E3" s="12">
         <v>0</v>
@@ -2949,13 +2837,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="12">
         <v>2</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E4" s="12">
         <v>0</v>
@@ -2972,13 +2860,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="12">
         <v>3</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E5" s="12">
         <v>0</v>
@@ -2992,7 +2880,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C6" s="12">
         <v>9</v>
@@ -3011,7 +2899,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3026,16 +2916,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3046,10 +2936,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3060,10 +2950,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3071,13 +2961,13 @@
         <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C4" s="10">
         <v>9</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3091,7 +2981,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3102,7 +2992,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F72AEC-DC8E-4753-A668-395BB0273289}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3112,105 +3002,95 @@
     <col min="2" max="2" width="25" style="10" customWidth="1"/>
     <col min="3" max="3" width="14" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="10" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="10" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="10"/>
+    <col min="5" max="5" width="16.7109375" style="10" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="10" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>86</v>
+        <v>230</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C2" s="10">
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E2" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="10">
         <v>0</v>
       </c>
-      <c r="H2" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C3" s="10">
         <v>2</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E3" s="10">
         <v>0</v>
       </c>
       <c r="F3" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="10">
-        <v>1</v>
-      </c>
-      <c r="H3" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C4" s="10">
         <v>3</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E4" s="10">
         <v>0</v>
@@ -3219,18 +3099,15 @@
         <v>0</v>
       </c>
       <c r="G4" s="10">
-        <v>0</v>
-      </c>
-      <c r="H4" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>7</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C5" s="10">
         <v>9</v>
@@ -3239,21 +3116,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>8</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C6" s="10">
         <v>0</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E6" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="10">
         <v>0</v>
@@ -3261,11 +3138,8 @@
       <c r="G6" s="10">
         <v>0</v>
       </c>
-      <c r="H6" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>9</v>
       </c>
@@ -3276,10 +3150,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>12</v>
       </c>
@@ -3287,7 +3161,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3314,19 +3188,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3334,13 +3208,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="12">
         <v>1</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="12">
         <v>1</v>
@@ -3351,13 +3225,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="12">
         <v>0</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="12">
         <v>0</v>
@@ -3374,7 +3248,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3388,7 +3262,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3398,75 +3272,86 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="12.42578125" style="12" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" style="12" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>26</v>
+        <v>227</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="12">
         <v>1</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="E2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="12">
         <v>0</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>9</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C4" s="12">
         <v>9</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3497,25 +3382,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3523,13 +3408,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="12">
         <v>0</v>
@@ -3546,13 +3431,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="12">
         <v>1</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="12">
         <v>1</v>
@@ -3566,13 +3451,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="C4" s="12">
         <v>2</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E4" s="12">
         <v>0</v>
@@ -3589,13 +3474,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="12">
         <v>4</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="E5" s="12">
         <v>0</v>
@@ -3612,13 +3497,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="12">
         <v>3</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="12">
         <v>0</v>
@@ -3635,13 +3520,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="12">
         <v>4</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="E7" s="12">
         <v>0</v>
@@ -3658,13 +3543,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="12">
         <v>4</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="E8" s="12">
         <v>0</v>
@@ -3681,13 +3566,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="12">
         <v>4</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="E9" s="12">
         <v>0</v>
@@ -3710,7 +3595,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3724,18 +3609,18 @@
         <v>9</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="12">
         <v>9</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3745,9 +3630,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3755,25 +3642,25 @@
     <col min="2" max="2" width="45.140625" style="12" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" style="12" customWidth="1"/>
-    <col min="5" max="8" width="7.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="12"/>
+    <col min="5" max="7" width="7.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>19</v>
@@ -3781,109 +3668,106 @@
       <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C2" s="12">
         <v>9</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C3" s="12">
         <v>9</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C4" s="12">
         <v>9</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C5" s="12">
         <v>9</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C6" s="12">
         <v>9</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C7" s="12">
         <v>9</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C8" s="12">
         <v>0</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E8" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="12">
         <v>0</v>
@@ -3891,25 +3775,22 @@
       <c r="G8" s="12">
         <v>0</v>
       </c>
-      <c r="H8" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C9" s="12">
         <v>0</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="E9" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="12">
         <v>0</v>
@@ -3917,126 +3798,111 @@
       <c r="G9" s="12">
         <v>0</v>
       </c>
-      <c r="H9" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C10" s="12">
         <v>1</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E10" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="12">
         <v>0</v>
       </c>
-      <c r="H10" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C11" s="12">
         <v>1</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E11" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="12">
         <v>0</v>
       </c>
-      <c r="H11" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C12" s="12">
         <v>2</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="E12" s="12">
         <v>0</v>
       </c>
       <c r="F12" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="12">
-        <v>1</v>
-      </c>
-      <c r="H12" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C13" s="12">
         <v>2</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="E13" s="12">
         <v>0</v>
       </c>
       <c r="F13" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="12">
-        <v>1</v>
-      </c>
-      <c r="H13" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C14" s="12">
         <v>3</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E14" s="12">
         <v>0</v>
@@ -4045,24 +3911,21 @@
         <v>0</v>
       </c>
       <c r="G14" s="12">
-        <v>0</v>
-      </c>
-      <c r="H14" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C15" s="12">
         <v>9</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -4073,11 +3936,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4086,52 +3947,48 @@
     <col min="3" max="3" width="12.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.42578125" style="12" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="12" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="12"/>
+    <col min="6" max="6" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.42578125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="12" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>175</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E2" s="12">
         <v>1</v>
@@ -4142,22 +3999,19 @@
       <c r="G2" s="12">
         <v>0</v>
       </c>
-      <c r="H2" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="12">
         <v>0</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E3" s="12">
         <v>1</v>
@@ -4168,22 +4022,19 @@
       <c r="G3" s="12">
         <v>0</v>
       </c>
-      <c r="H3" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" s="12">
         <v>0</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E4" s="12">
         <v>1</v>
@@ -4194,74 +4045,65 @@
       <c r="G4" s="12">
         <v>0</v>
       </c>
-      <c r="H4" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5" s="12">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" s="12">
         <v>0</v>
       </c>
       <c r="F5" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="12">
         <v>0</v>
       </c>
-      <c r="H5" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="12">
         <v>2</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="12">
         <v>0</v>
       </c>
       <c r="F6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="12">
-        <v>1</v>
-      </c>
-      <c r="H6" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" s="12">
         <v>3</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="12">
         <v>0</v>
@@ -4270,13 +4112,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="12">
-        <v>0</v>
-      </c>
-      <c r="H7" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>9</v>
       </c>
@@ -4287,23 +4126,23 @@
         <v>9</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K19" s="5"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -4313,11 +4152,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4325,51 +4162,48 @@
     <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="8" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="22" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="22" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" s="12">
         <v>0</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="E2" s="12">
         <v>1</v>
@@ -4383,22 +4217,19 @@
       <c r="H2" s="12">
         <v>0</v>
       </c>
-      <c r="I2" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="12">
         <v>0</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="E3" s="12">
         <v>1</v>
@@ -4412,22 +4243,19 @@
       <c r="H3" s="12">
         <v>0</v>
       </c>
-      <c r="I3" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="12">
         <v>1</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="E4" s="12">
         <v>0</v>
@@ -4441,22 +4269,19 @@
       <c r="H4" s="12">
         <v>0</v>
       </c>
-      <c r="I4" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" s="12">
         <v>1</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="E5" s="12">
         <v>0</v>
@@ -4470,22 +4295,19 @@
       <c r="H5" s="12">
         <v>1</v>
       </c>
-      <c r="I5" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" s="12">
         <v>2</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="E6" s="12">
         <v>0</v>
@@ -4499,22 +4321,19 @@
       <c r="H6" s="12">
         <v>0</v>
       </c>
-      <c r="I6" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" s="12">
         <v>3</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E7" s="12">
         <v>0</v>
@@ -4528,22 +4347,19 @@
       <c r="H7" s="12">
         <v>1</v>
       </c>
-      <c r="I7" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8" s="12">
         <v>4</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="E8" s="12">
         <v>0</v>
@@ -4557,22 +4373,19 @@
       <c r="H8" s="12">
         <v>0</v>
       </c>
-      <c r="I8" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" s="12">
         <v>4</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="E9" s="12">
         <v>0</v>
@@ -4586,30 +4399,26 @@
       <c r="H9" s="12">
         <v>0</v>
       </c>
-      <c r="I9" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>77</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" s="12">
         <v>9</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>99</v>
       </c>
@@ -4620,13 +4429,12 @@
         <v>9</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add and publish descriptive analysis
</commit_message>
<xml_diff>
--- a/output/Data_Dictionary.xlsx
+++ b/output/Data_Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RProjects\github\toothheart\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742844D7-8D59-4E49-870A-81BB4503DFB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6CD782-F8BA-4EE4-82B8-D4ECE9E71CA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="780" windowWidth="25980" windowHeight="14385" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="1125" windowWidth="25980" windowHeight="14385" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="235">
   <si>
     <t>Fieldname</t>
   </si>
@@ -757,6 +757,15 @@
   </si>
   <si>
     <t>SOMECOLl</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>"Y</t>
   </si>
 </sst>
 </file>
@@ -2715,8 +2724,8 @@
       <c r="B4" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="12">
-        <v>9</v>
+      <c r="C4" s="12" t="s">
+        <v>234</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>127</v>
@@ -3956,7 +3965,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>40</v>
+        <v>232</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
@@ -4154,7 +4163,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4168,7 +4179,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="22" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>44</v>
+        <v>233</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>

</xml_diff>